<commit_message>
functionality is here now
</commit_message>
<xml_diff>
--- a/testres/asdasd.xlsx
+++ b/testres/asdasd.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -26,6 +26,9 @@
     <t>adress</t>
   </si>
   <si>
+    <t>phone</t>
+  </si>
+  <si>
     <t>Bauer</t>
   </si>
   <si>
@@ -38,6 +41,9 @@
     <t>Bauerweg 18</t>
   </si>
   <si>
+    <t>2.020202E7</t>
+  </si>
+  <si>
     <t>Lang</t>
   </si>
   <si>
@@ -48,6 +54,39 @@
   </si>
   <si>
     <t>Drehstr. 15</t>
+  </si>
+  <si>
+    <t>6.060606E7</t>
+  </si>
+  <si>
+    <t>Hecht</t>
+  </si>
+  <si>
+    <t>Felix</t>
+  </si>
+  <si>
+    <t>Felixderdiggeplaya@googlemail.com</t>
+  </si>
+  <si>
+    <t>AndyStr 5</t>
+  </si>
+  <si>
+    <t>5050505.0</t>
+  </si>
+  <si>
+    <t>Newel</t>
+  </si>
+  <si>
+    <t>Gabe</t>
+  </si>
+  <si>
+    <t>Hl3.confirmed@gmx.net</t>
+  </si>
+  <si>
+    <t>California dreamin</t>
+  </si>
+  <si>
+    <t>3.03030303E8</t>
   </si>
 </sst>
 </file>
@@ -111,33 +150,76 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>